<commit_message>
Refactor architecture and enhance documentation for steady-state evolution
- Updated ARCHITECTURE.md to reflect the transition to a steady-state population management system, detailing the new elite preservation strategy and the introduction of `elites.json`.
- Revised README.md and design_document.md to include recent enhancements, such as the comprehensive suite of 16 text variation operators and multi-language support.
- Adjusted file handling in the codebase to accommodate the new steady-state logic, ensuring compatibility with existing workflows.
- Removed obsolete files and updated paths to streamline the project structure and improve maintainability.
</commit_message>
<xml_diff>
--- a/data/elite_count_by_generation.xlsx
+++ b/data/elite_count_by_generation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>1</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" t="n">
         <v>1</v>
@@ -471,15 +471,15 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B7" t="n">
         <v>2</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B8" t="n">
         <v>1</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -519,15 +519,15 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" t="n">
         <v>1</v>
@@ -535,23 +535,23 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B15" t="n">
         <v>1</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B16" t="n">
         <v>1</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" t="n">
         <v>1</v>
@@ -575,15 +575,15 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B19" t="n">
         <v>2</v>
@@ -591,15 +591,15 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B21" t="n">
         <v>2</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B22" t="n">
         <v>1</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B23" t="n">
         <v>1</v>
@@ -623,31 +623,31 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B27" t="n">
         <v>1</v>
@@ -655,7 +655,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" t="n">
         <v>2</v>
@@ -663,15 +663,15 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B30" t="n">
         <v>1</v>
@@ -679,23 +679,23 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B33" t="n">
         <v>1</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B34" t="n">
         <v>1</v>
@@ -711,7 +711,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B35" t="n">
         <v>2</v>
@@ -719,7 +719,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B36" t="n">
         <v>1</v>
@@ -727,15 +727,15 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B38" t="n">
         <v>2</v>
@@ -743,23 +743,23 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B39" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B40" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B41" t="n">
         <v>3</v>
@@ -767,23 +767,23 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B42" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B44" t="n">
         <v>1</v>
@@ -791,7 +791,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B45" t="n">
         <v>1</v>
@@ -799,130 +799,82 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B46" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B48" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B50" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B52" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B54" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>101</v>
-      </c>
-      <c r="B56" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>102</v>
-      </c>
-      <c r="B57" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>103</v>
-      </c>
-      <c r="B58" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>105</v>
-      </c>
-      <c r="B59" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>106</v>
-      </c>
-      <c r="B60" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>110</v>
-      </c>
-      <c r="B61" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>